<commit_message>
Add Excel and images updated
</commit_message>
<xml_diff>
--- a/noprofit/en/11255/inpag-template.xlsx
+++ b/noprofit/en/11255/inpag-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrick.pasquillo\Documents\GitHub\Universal\noprofit\en\11255\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AA23B2-D226-46C1-97C1-0C1CEF0A1F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA20E27-1C79-401B-9F4F-65F1E594FB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="692" xr2:uid="{8907ADCE-C3F1-4516-963F-08DDED88069F}"/>
   </bookViews>
@@ -1360,6 +1360,15 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1372,15 +1381,6 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1405,47 +1405,47 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2162,6 +2162,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B10:G16"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B20:G20"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="B27:G27"/>
@@ -2178,12 +2184,6 @@
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B10:G16"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="51" orientation="portrait" r:id="rId1"/>
@@ -2200,8 +2200,8 @@
   </sheetPr>
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2217,84 +2217,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
     </row>
     <row r="2" spans="1:5" ht="36" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="108" t="str">
+      <c r="B2" s="104" t="str">
         <f>'General information'!B2</f>
         <v>No-ProfitName LegalForm</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="108" t="str">
+      <c r="B3" s="104" t="str">
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="110">
+      <c r="B4" s="106">
         <f>'General information'!B8</f>
         <v>45292</v>
       </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="110">
+      <c r="B5" s="106">
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
     </row>
     <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="107" t="s">
         <v>269</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
+      <c r="A7" s="107"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="104"/>
-      <c r="B8" s="104"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
@@ -2317,12 +2317,12 @@
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="107"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
@@ -2416,12 +2416,12 @@
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="107"/>
-      <c r="D17" s="107"/>
-      <c r="E17" s="107"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="110"/>
     </row>
     <row r="18" spans="1:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
@@ -2549,12 +2549,12 @@
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="44"/>
-      <c r="B26" s="107" t="s">
+      <c r="B26" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="107"/>
-      <c r="D26" s="107"/>
-      <c r="E26" s="107"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
     </row>
     <row r="27" spans="1:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="s">
@@ -2682,12 +2682,12 @@
     </row>
     <row r="35" spans="1:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="44"/>
-      <c r="B35" s="107" t="s">
+      <c r="B35" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="107"/>
-      <c r="D35" s="107"/>
-      <c r="E35" s="107"/>
+      <c r="C35" s="110"/>
+      <c r="D35" s="110"/>
+      <c r="E35" s="110"/>
     </row>
     <row r="36" spans="1:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="44" t="s">
@@ -2764,12 +2764,12 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="44"/>
-      <c r="B41" s="107" t="s">
+      <c r="B41" s="110" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="107"/>
-      <c r="D41" s="107"/>
-      <c r="E41" s="107"/>
+      <c r="C41" s="110"/>
+      <c r="D41" s="110"/>
+      <c r="E41" s="110"/>
     </row>
     <row r="42" spans="1:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="44" t="s">
@@ -2892,10 +2892,10 @@
     </row>
     <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="44"/>
-      <c r="B49" s="107" t="s">
+      <c r="B49" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="C49" s="107"/>
+      <c r="C49" s="110"/>
       <c r="D49" s="62">
         <f>SUM(D42:D48)</f>
         <v>0</v>
@@ -2907,10 +2907,10 @@
     </row>
     <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="44"/>
-      <c r="B50" s="107" t="s">
+      <c r="B50" s="110" t="s">
         <v>74</v>
       </c>
-      <c r="C50" s="107"/>
+      <c r="C50" s="110"/>
       <c r="D50" s="62">
         <f>SUM(D33,D39,D49)</f>
         <v>0</v>
@@ -2938,11 +2938,11 @@
       <c r="A53" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="106" t="str">
+      <c r="B53" s="109" t="str">
         <f>IF((D15+D23+D33=D39+D49),"Ok","Attention! The total liabilities do not match the total assets!")</f>
         <v>Ok</v>
       </c>
-      <c r="C53" s="106"/>
+      <c r="C53" s="109"/>
       <c r="D53" s="53">
         <f>D50-D23</f>
         <v>0</v>
@@ -2952,12 +2952,12 @@
       <c r="A54" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="B54" s="105" t="str">
+      <c r="B54" s="108" t="str">
         <f>IF((E15+E23+E33=E39+E49),"Ok","Attention! The total liabilities do not match the total assets!")</f>
         <v>Ok</v>
       </c>
-      <c r="C54" s="105"/>
-      <c r="D54" s="105"/>
+      <c r="C54" s="108"/>
+      <c r="D54" s="108"/>
       <c r="E54" s="53">
         <f>E50-E23</f>
         <v>0</v>
@@ -2971,11 +2971,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
     <mergeCell ref="A6:E8"/>
     <mergeCell ref="B54:D54"/>
     <mergeCell ref="B53:C53"/>
@@ -2986,6 +2981,11 @@
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B53">
@@ -3026,8 +3026,8 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection sqref="A1:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3103,27 +3103,27 @@
       <c r="E5" s="113"/>
     </row>
     <row r="6" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="107" t="s">
         <v>268</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
+      <c r="A7" s="107"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
     </row>
     <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="104"/>
-      <c r="B8" s="104"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
     </row>
     <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="74" t="s">
@@ -3708,13 +3708,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
@@ -3723,72 +3723,72 @@
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="108" t="str">
+      <c r="B2" s="104" t="str">
         <f>'General information'!B2</f>
         <v>No-ProfitName LegalForm</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="108" t="str">
+      <c r="B3" s="104" t="str">
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="110">
+      <c r="B4" s="106">
         <f>'General information'!B8</f>
         <v>45292</v>
       </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="110">
+      <c r="B5" s="106">
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="107" t="s">
         <v>256</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="104"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
+      <c r="A7" s="107"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="104"/>
-      <c r="B8" s="104"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="74" t="s">
@@ -4007,11 +4007,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="A6:E8"/>
     <mergeCell ref="B25:D25"/>
@@ -4024,6 +4019,11 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="79" orientation="landscape" r:id="rId1"/>
@@ -4055,94 +4055,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="108" t="str">
+      <c r="B2" s="104" t="str">
         <f>'General information'!B2</f>
         <v>No-ProfitName LegalForm</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="108" t="str">
+      <c r="B3" s="104" t="str">
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
     </row>
     <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="110">
+      <c r="B4" s="106">
         <f>'General information'!B8</f>
         <v>45292</v>
       </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="110">
+      <c r="B5" s="106">
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
     </row>
     <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="107" t="s">
         <v>267</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
+      <c r="A7" s="107"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="104"/>
-      <c r="B8" s="104"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="120" t="s">
+      <c r="B9" s="119" t="s">
         <v>167</v>
       </c>
-      <c r="C9" s="120"/>
+      <c r="C9" s="119"/>
       <c r="D9" s="74" t="s">
         <v>27</v>
       </c>
@@ -4155,11 +4155,11 @@
       <c r="A10" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="110" t="s">
         <v>168</v>
       </c>
-      <c r="C10" s="107"/>
-      <c r="D10" s="107"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
       <c r="E10" s="22">
         <v>0</v>
       </c>
@@ -4175,10 +4175,10 @@
       <c r="A12" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="120" t="s">
+      <c r="B12" s="119" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="120"/>
+      <c r="C12" s="119"/>
       <c r="D12" s="74" t="s">
         <v>27</v>
       </c>
@@ -4300,10 +4300,10 @@
       <c r="A21" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="B21" s="119" t="s">
+      <c r="B21" s="120" t="s">
         <v>243</v>
       </c>
-      <c r="C21" s="119"/>
+      <c r="C21" s="120"/>
       <c r="D21" s="90"/>
       <c r="E21" s="22">
         <v>0</v>
@@ -4314,10 +4314,10 @@
       <c r="A22" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="B22" s="119" t="s">
+      <c r="B22" s="120" t="s">
         <v>244</v>
       </c>
-      <c r="C22" s="119"/>
+      <c r="C22" s="120"/>
       <c r="D22" s="90"/>
       <c r="E22" s="22">
         <v>0</v>
@@ -4328,10 +4328,10 @@
       <c r="A23" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="B23" s="119" t="s">
+      <c r="B23" s="120" t="s">
         <v>245</v>
       </c>
-      <c r="C23" s="119"/>
+      <c r="C23" s="120"/>
       <c r="D23" s="90"/>
       <c r="E23" s="22">
         <v>0</v>
@@ -4342,10 +4342,10 @@
       <c r="A24" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="B24" s="119" t="s">
+      <c r="B24" s="120" t="s">
         <v>246</v>
       </c>
-      <c r="C24" s="119"/>
+      <c r="C24" s="120"/>
       <c r="D24" s="90"/>
       <c r="E24" s="22">
         <v>0</v>
@@ -4354,11 +4354,11 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
-      <c r="B25" s="107" t="s">
+      <c r="B25" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="107"/>
-      <c r="D25" s="107"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="110"/>
       <c r="E25" s="62">
         <f>E10+SUM(E13:E24)</f>
         <v>0</v>
@@ -4375,10 +4375,10 @@
       <c r="A27" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="120" t="s">
+      <c r="B27" s="119" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="120"/>
+      <c r="C27" s="119"/>
       <c r="D27" s="74" t="s">
         <v>27</v>
       </c>
@@ -4391,10 +4391,10 @@
       <c r="A28" s="44" t="s">
         <v>190</v>
       </c>
-      <c r="B28" s="119" t="s">
+      <c r="B28" s="120" t="s">
         <v>253</v>
       </c>
-      <c r="C28" s="119"/>
+      <c r="C28" s="120"/>
       <c r="D28" s="90"/>
       <c r="E28" s="22">
         <v>0</v>
@@ -4404,10 +4404,10 @@
       <c r="A29" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="B29" s="119" t="s">
+      <c r="B29" s="120" t="s">
         <v>254</v>
       </c>
-      <c r="C29" s="119"/>
+      <c r="C29" s="120"/>
       <c r="D29" s="90"/>
       <c r="E29" s="22">
         <v>0</v>
@@ -4417,10 +4417,10 @@
       <c r="A30" s="44" t="s">
         <v>192</v>
       </c>
-      <c r="B30" s="119" t="s">
+      <c r="B30" s="120" t="s">
         <v>248</v>
       </c>
-      <c r="C30" s="119"/>
+      <c r="C30" s="120"/>
       <c r="D30" s="90"/>
       <c r="E30" s="22">
         <v>0</v>
@@ -4430,10 +4430,10 @@
       <c r="A31" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="B31" s="119" t="s">
+      <c r="B31" s="120" t="s">
         <v>255</v>
       </c>
-      <c r="C31" s="119"/>
+      <c r="C31" s="120"/>
       <c r="D31" s="90"/>
       <c r="E31" s="22">
         <v>0</v>
@@ -4441,11 +4441,11 @@
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="44"/>
-      <c r="B32" s="107" t="s">
+      <c r="B32" s="110" t="s">
         <v>116</v>
       </c>
-      <c r="C32" s="107"/>
-      <c r="D32" s="107"/>
+      <c r="C32" s="110"/>
+      <c r="D32" s="110"/>
       <c r="E32" s="62">
         <f>E10+E25+SUM(E28:E31)</f>
         <v>0</v>
@@ -4462,10 +4462,10 @@
       <c r="A34" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="120" t="s">
+      <c r="B34" s="119" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="120"/>
+      <c r="C34" s="119"/>
       <c r="D34" s="74" t="s">
         <v>27</v>
       </c>
@@ -4479,10 +4479,10 @@
       <c r="A35" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="B35" s="119" t="s">
+      <c r="B35" s="120" t="s">
         <v>249</v>
       </c>
-      <c r="C35" s="119"/>
+      <c r="C35" s="120"/>
       <c r="D35" s="90"/>
       <c r="E35" s="22">
         <v>0</v>
@@ -4492,10 +4492,10 @@
       <c r="A36" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="B36" s="119" t="s">
+      <c r="B36" s="120" t="s">
         <v>250</v>
       </c>
-      <c r="C36" s="119"/>
+      <c r="C36" s="120"/>
       <c r="D36" s="90"/>
       <c r="E36" s="22">
         <v>0</v>
@@ -4505,10 +4505,10 @@
       <c r="A37" s="44" t="s">
         <v>196</v>
       </c>
-      <c r="B37" s="119" t="s">
+      <c r="B37" s="120" t="s">
         <v>251</v>
       </c>
-      <c r="C37" s="119"/>
+      <c r="C37" s="120"/>
       <c r="D37" s="90"/>
       <c r="E37" s="22">
         <v>0</v>
@@ -4516,11 +4516,11 @@
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="44"/>
-      <c r="B38" s="107" t="s">
+      <c r="B38" s="110" t="s">
         <v>118</v>
       </c>
-      <c r="C38" s="107"/>
-      <c r="D38" s="107"/>
+      <c r="C38" s="110"/>
+      <c r="D38" s="110"/>
       <c r="E38" s="62">
         <f>E10+E25+E32+SUM(E35:E37)</f>
         <v>0</v>
@@ -4535,11 +4535,11 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="44"/>
-      <c r="B40" s="107" t="s">
+      <c r="B40" s="110" t="s">
         <v>119</v>
       </c>
-      <c r="C40" s="107"/>
-      <c r="D40" s="107"/>
+      <c r="C40" s="110"/>
+      <c r="D40" s="110"/>
       <c r="E40" s="62">
         <f>SUM(E25,E32,E38)</f>
         <v>0</v>
@@ -4593,10 +4593,10 @@
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="44"/>
-      <c r="B45" s="107" t="s">
+      <c r="B45" s="110" t="s">
         <v>120</v>
       </c>
-      <c r="C45" s="107"/>
+      <c r="C45" s="110"/>
       <c r="D45" s="93">
         <v>49</v>
       </c>
@@ -4607,11 +4607,11 @@
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="44"/>
-      <c r="B46" s="107" t="s">
+      <c r="B46" s="110" t="s">
         <v>121</v>
       </c>
-      <c r="C46" s="107"/>
-      <c r="D46" s="107"/>
+      <c r="C46" s="110"/>
+      <c r="D46" s="110"/>
       <c r="E46" s="69">
         <f>'Statement of Financial Position'!D22</f>
         <v>0</v>
@@ -4619,11 +4619,11 @@
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="44"/>
-      <c r="B47" s="107" t="s">
+      <c r="B47" s="110" t="s">
         <v>122</v>
       </c>
-      <c r="C47" s="107"/>
-      <c r="D47" s="107"/>
+      <c r="C47" s="110"/>
+      <c r="D47" s="110"/>
       <c r="E47" s="69">
         <f>'Statement of Financial Position'!E22</f>
         <v>0</v>
@@ -4631,11 +4631,11 @@
     </row>
     <row r="48" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A48" s="44"/>
-      <c r="B48" s="107" t="s">
+      <c r="B48" s="110" t="s">
         <v>123</v>
       </c>
-      <c r="C48" s="107"/>
-      <c r="D48" s="107"/>
+      <c r="C48" s="110"/>
+      <c r="D48" s="110"/>
       <c r="E48" s="69">
         <f>E47-E46</f>
         <v>0</v>
@@ -4735,25 +4735,18 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A6:E8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B32:D32"/>
@@ -4770,18 +4763,25 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A6:E8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" orientation="portrait" r:id="rId1"/>
@@ -4812,85 +4812,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="121" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="108" t="str">
+      <c r="B2" s="104" t="str">
         <f>'General information'!B2</f>
         <v>No-ProfitName LegalForm</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="108" t="str">
+      <c r="B3" s="104" t="str">
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="110">
+      <c r="B4" s="106">
         <f>'General information'!B8</f>
         <v>45292</v>
       </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="110">
+      <c r="B5" s="106">
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
     </row>
     <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="107" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
+      <c r="A7" s="107"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
     </row>
     <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="104"/>
-      <c r="B8" s="104"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="125" t="s">
+      <c r="A9" s="123" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="125"/>
-      <c r="C9" s="125"/>
-      <c r="D9" s="125"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="123"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="122"/>
@@ -4911,34 +4911,34 @@
       <c r="D12" s="122"/>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="123"/>
-      <c r="B13" s="123"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
+      <c r="A13" s="124"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="124"/>
+      <c r="D13" s="124"/>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="123"/>
-      <c r="B14" s="123"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
+      <c r="A14" s="124"/>
+      <c r="B14" s="124"/>
+      <c r="C14" s="124"/>
+      <c r="D14" s="124"/>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="123"/>
-      <c r="B15" s="123"/>
-      <c r="C15" s="123"/>
-      <c r="D15" s="123"/>
+      <c r="A15" s="124"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="123"/>
-      <c r="B16" s="123"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="123"/>
+      <c r="A16" s="124"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="124"/>
+      <c r="D16" s="124"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="123"/>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="123"/>
+      <c r="A17" s="124"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="124"/>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="122"/>
@@ -5007,10 +5007,10 @@
       <c r="D28" s="122"/>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="121"/>
-      <c r="B29" s="121"/>
-      <c r="C29" s="121"/>
-      <c r="D29" s="121"/>
+      <c r="A29" s="125"/>
+      <c r="B29" s="125"/>
+      <c r="C29" s="125"/>
+      <c r="D29" s="125"/>
     </row>
     <row r="30" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
@@ -5640,6 +5640,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A19:D19"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A24:D24"/>
@@ -5655,18 +5667,6 @@
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A19:D19"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5713,65 +5713,65 @@
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="108" t="str">
+      <c r="B2" s="104" t="str">
         <f>'General information'!B2</f>
         <v>No-ProfitName LegalForm</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="108" t="str">
+      <c r="B3" s="104" t="str">
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="110">
+      <c r="B4" s="106">
         <f>'General information'!B8</f>
         <v>45292</v>
       </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="110">
+      <c r="B5" s="106">
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
     </row>
     <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="107" t="s">
         <v>266</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
+      <c r="A7" s="107"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="104"/>
-      <c r="B8" s="104"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -6281,48 +6281,48 @@
       <c r="L5" s="131"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="127" t="s">
+      <c r="A6" s="132" t="s">
         <v>265</v>
       </c>
-      <c r="B6" s="127"/>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
+      <c r="B6" s="132"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
     </row>
     <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="127"/>
-      <c r="B7" s="127"/>
-      <c r="C7" s="127"/>
-      <c r="D7" s="127"/>
-      <c r="E7" s="127"/>
-      <c r="F7" s="127"/>
-      <c r="G7" s="127"/>
-      <c r="H7" s="127"/>
-      <c r="I7" s="127"/>
-      <c r="J7" s="127"/>
-      <c r="K7" s="127"/>
-      <c r="L7" s="127"/>
+      <c r="A7" s="132"/>
+      <c r="B7" s="132"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="132"/>
+      <c r="K7" s="132"/>
+      <c r="L7" s="132"/>
     </row>
     <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="127"/>
-      <c r="B8" s="127"/>
-      <c r="C8" s="127"/>
-      <c r="D8" s="127"/>
-      <c r="E8" s="127"/>
-      <c r="F8" s="127"/>
-      <c r="G8" s="127"/>
-      <c r="H8" s="127"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="127"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="127"/>
+      <c r="A8" s="132"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
+      <c r="K8" s="132"/>
+      <c r="L8" s="132"/>
     </row>
     <row r="9" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="78" t="s">
@@ -6334,17 +6334,17 @@
       <c r="C9" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="129" t="s">
+      <c r="D9" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="129"/>
-      <c r="F9" s="129"/>
-      <c r="G9" s="129"/>
-      <c r="H9" s="129"/>
-      <c r="I9" s="129"/>
-      <c r="J9" s="129"/>
-      <c r="K9" s="129"/>
-      <c r="L9" s="129"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="128"/>
+      <c r="J9" s="128"/>
+      <c r="K9" s="128"/>
+      <c r="L9" s="128"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="97"/>
@@ -6352,15 +6352,15 @@
       <c r="C10" s="81">
         <v>0</v>
       </c>
-      <c r="D10" s="128"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="128"/>
-      <c r="G10" s="128"/>
-      <c r="H10" s="128"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
-      <c r="K10" s="128"/>
-      <c r="L10" s="128"/>
+      <c r="D10" s="127"/>
+      <c r="E10" s="127"/>
+      <c r="F10" s="127"/>
+      <c r="G10" s="127"/>
+      <c r="H10" s="127"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="127"/>
+      <c r="K10" s="127"/>
+      <c r="L10" s="127"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="97"/>
@@ -6368,15 +6368,15 @@
       <c r="C11" s="81">
         <v>0</v>
       </c>
-      <c r="D11" s="128"/>
-      <c r="E11" s="128"/>
-      <c r="F11" s="128"/>
-      <c r="G11" s="128"/>
-      <c r="H11" s="128"/>
-      <c r="I11" s="128"/>
-      <c r="J11" s="128"/>
-      <c r="K11" s="128"/>
-      <c r="L11" s="128"/>
+      <c r="D11" s="127"/>
+      <c r="E11" s="127"/>
+      <c r="F11" s="127"/>
+      <c r="G11" s="127"/>
+      <c r="H11" s="127"/>
+      <c r="I11" s="127"/>
+      <c r="J11" s="127"/>
+      <c r="K11" s="127"/>
+      <c r="L11" s="127"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="97"/>
@@ -6384,15 +6384,15 @@
       <c r="C12" s="81">
         <v>0</v>
       </c>
-      <c r="D12" s="128"/>
-      <c r="E12" s="128"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="128"/>
-      <c r="H12" s="128"/>
-      <c r="I12" s="128"/>
-      <c r="J12" s="128"/>
-      <c r="K12" s="128"/>
-      <c r="L12" s="128"/>
+      <c r="D12" s="127"/>
+      <c r="E12" s="127"/>
+      <c r="F12" s="127"/>
+      <c r="G12" s="127"/>
+      <c r="H12" s="127"/>
+      <c r="I12" s="127"/>
+      <c r="J12" s="127"/>
+      <c r="K12" s="127"/>
+      <c r="L12" s="127"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="77">
@@ -6439,17 +6439,17 @@
       <c r="C15" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="D15" s="129" t="s">
+      <c r="D15" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="129"/>
-      <c r="F15" s="129"/>
-      <c r="G15" s="129"/>
-      <c r="H15" s="129"/>
-      <c r="I15" s="129"/>
-      <c r="J15" s="129"/>
-      <c r="K15" s="129"/>
-      <c r="L15" s="129"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="128"/>
+      <c r="G15" s="128"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="128"/>
+      <c r="K15" s="128"/>
+      <c r="L15" s="128"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="97"/>
@@ -6457,15 +6457,15 @@
       <c r="C16" s="81">
         <v>0</v>
       </c>
-      <c r="D16" s="128"/>
-      <c r="E16" s="128"/>
-      <c r="F16" s="128"/>
-      <c r="G16" s="128"/>
-      <c r="H16" s="128"/>
-      <c r="I16" s="128"/>
-      <c r="J16" s="128"/>
-      <c r="K16" s="128"/>
-      <c r="L16" s="128"/>
+      <c r="D16" s="127"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="127"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="127"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="127"/>
+      <c r="L16" s="127"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="97"/>
@@ -6473,15 +6473,15 @@
       <c r="C17" s="81">
         <v>0</v>
       </c>
-      <c r="D17" s="128"/>
-      <c r="E17" s="128"/>
-      <c r="F17" s="128"/>
-      <c r="G17" s="128"/>
-      <c r="H17" s="128"/>
-      <c r="I17" s="128"/>
-      <c r="J17" s="128"/>
-      <c r="K17" s="128"/>
-      <c r="L17" s="128"/>
+      <c r="D17" s="127"/>
+      <c r="E17" s="127"/>
+      <c r="F17" s="127"/>
+      <c r="G17" s="127"/>
+      <c r="H17" s="127"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="127"/>
+      <c r="K17" s="127"/>
+      <c r="L17" s="127"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="97"/>
@@ -6489,15 +6489,15 @@
       <c r="C18" s="81">
         <v>0</v>
       </c>
-      <c r="D18" s="128"/>
-      <c r="E18" s="128"/>
-      <c r="F18" s="128"/>
-      <c r="G18" s="128"/>
-      <c r="H18" s="128"/>
-      <c r="I18" s="128"/>
-      <c r="J18" s="128"/>
-      <c r="K18" s="128"/>
-      <c r="L18" s="128"/>
+      <c r="D18" s="127"/>
+      <c r="E18" s="127"/>
+      <c r="F18" s="127"/>
+      <c r="G18" s="127"/>
+      <c r="H18" s="127"/>
+      <c r="I18" s="127"/>
+      <c r="J18" s="127"/>
+      <c r="K18" s="127"/>
+      <c r="L18" s="127"/>
     </row>
     <row r="19" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="77">
@@ -6544,17 +6544,17 @@
       <c r="C21" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="D21" s="129" t="s">
+      <c r="D21" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="129"/>
-      <c r="F21" s="129"/>
-      <c r="G21" s="129"/>
-      <c r="H21" s="129"/>
-      <c r="I21" s="129"/>
-      <c r="J21" s="129"/>
-      <c r="K21" s="129"/>
-      <c r="L21" s="129"/>
+      <c r="E21" s="128"/>
+      <c r="F21" s="128"/>
+      <c r="G21" s="128"/>
+      <c r="H21" s="128"/>
+      <c r="I21" s="128"/>
+      <c r="J21" s="128"/>
+      <c r="K21" s="128"/>
+      <c r="L21" s="128"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="97"/>
@@ -6562,15 +6562,15 @@
       <c r="C22" s="81">
         <v>0</v>
       </c>
-      <c r="D22" s="128"/>
-      <c r="E22" s="128"/>
-      <c r="F22" s="128"/>
-      <c r="G22" s="128"/>
-      <c r="H22" s="128"/>
-      <c r="I22" s="128"/>
-      <c r="J22" s="128"/>
-      <c r="K22" s="128"/>
-      <c r="L22" s="128"/>
+      <c r="D22" s="127"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="127"/>
+      <c r="I22" s="127"/>
+      <c r="J22" s="127"/>
+      <c r="K22" s="127"/>
+      <c r="L22" s="127"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="97"/>
@@ -6578,15 +6578,15 @@
       <c r="C23" s="81">
         <v>0</v>
       </c>
-      <c r="D23" s="128"/>
-      <c r="E23" s="128"/>
-      <c r="F23" s="128"/>
-      <c r="G23" s="128"/>
-      <c r="H23" s="128"/>
-      <c r="I23" s="128"/>
-      <c r="J23" s="128"/>
-      <c r="K23" s="128"/>
-      <c r="L23" s="128"/>
+      <c r="D23" s="127"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="127"/>
+      <c r="I23" s="127"/>
+      <c r="J23" s="127"/>
+      <c r="K23" s="127"/>
+      <c r="L23" s="127"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="97"/>
@@ -6594,15 +6594,15 @@
       <c r="C24" s="81">
         <v>0</v>
       </c>
-      <c r="D24" s="128"/>
-      <c r="E24" s="128"/>
-      <c r="F24" s="128"/>
-      <c r="G24" s="128"/>
-      <c r="H24" s="128"/>
-      <c r="I24" s="128"/>
-      <c r="J24" s="128"/>
-      <c r="K24" s="128"/>
-      <c r="L24" s="128"/>
+      <c r="D24" s="127"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="127"/>
+      <c r="G24" s="127"/>
+      <c r="H24" s="127"/>
+      <c r="I24" s="127"/>
+      <c r="J24" s="127"/>
+      <c r="K24" s="127"/>
+      <c r="L24" s="127"/>
     </row>
     <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="77">
@@ -6649,17 +6649,17 @@
       <c r="C27" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="129" t="s">
+      <c r="D27" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="129"/>
-      <c r="F27" s="129"/>
-      <c r="G27" s="129"/>
-      <c r="H27" s="129"/>
-      <c r="I27" s="129"/>
-      <c r="J27" s="129"/>
-      <c r="K27" s="129"/>
-      <c r="L27" s="129"/>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="128"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="128"/>
+      <c r="L27" s="128"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="97"/>
@@ -6667,15 +6667,15 @@
       <c r="C28" s="81">
         <v>0</v>
       </c>
-      <c r="D28" s="128"/>
-      <c r="E28" s="128"/>
-      <c r="F28" s="128"/>
-      <c r="G28" s="128"/>
-      <c r="H28" s="128"/>
-      <c r="I28" s="128"/>
-      <c r="J28" s="128"/>
-      <c r="K28" s="128"/>
-      <c r="L28" s="128"/>
+      <c r="D28" s="127"/>
+      <c r="E28" s="127"/>
+      <c r="F28" s="127"/>
+      <c r="G28" s="127"/>
+      <c r="H28" s="127"/>
+      <c r="I28" s="127"/>
+      <c r="J28" s="127"/>
+      <c r="K28" s="127"/>
+      <c r="L28" s="127"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="97"/>
@@ -6683,15 +6683,15 @@
       <c r="C29" s="81">
         <v>0</v>
       </c>
-      <c r="D29" s="128"/>
-      <c r="E29" s="128"/>
-      <c r="F29" s="128"/>
-      <c r="G29" s="128"/>
-      <c r="H29" s="128"/>
-      <c r="I29" s="128"/>
-      <c r="J29" s="128"/>
-      <c r="K29" s="128"/>
-      <c r="L29" s="128"/>
+      <c r="D29" s="127"/>
+      <c r="E29" s="127"/>
+      <c r="F29" s="127"/>
+      <c r="G29" s="127"/>
+      <c r="H29" s="127"/>
+      <c r="I29" s="127"/>
+      <c r="J29" s="127"/>
+      <c r="K29" s="127"/>
+      <c r="L29" s="127"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="97"/>
@@ -6699,15 +6699,15 @@
       <c r="C30" s="81">
         <v>0</v>
       </c>
-      <c r="D30" s="128"/>
-      <c r="E30" s="128"/>
-      <c r="F30" s="128"/>
-      <c r="G30" s="128"/>
-      <c r="H30" s="128"/>
-      <c r="I30" s="128"/>
-      <c r="J30" s="128"/>
-      <c r="K30" s="128"/>
-      <c r="L30" s="128"/>
+      <c r="D30" s="127"/>
+      <c r="E30" s="127"/>
+      <c r="F30" s="127"/>
+      <c r="G30" s="127"/>
+      <c r="H30" s="127"/>
+      <c r="I30" s="127"/>
+      <c r="J30" s="127"/>
+      <c r="K30" s="127"/>
+      <c r="L30" s="127"/>
     </row>
     <row r="31" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="77">
@@ -6754,17 +6754,17 @@
       <c r="C33" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="D33" s="129" t="s">
+      <c r="D33" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="E33" s="129"/>
-      <c r="F33" s="129"/>
-      <c r="G33" s="129"/>
-      <c r="H33" s="129"/>
-      <c r="I33" s="129"/>
-      <c r="J33" s="129"/>
-      <c r="K33" s="129"/>
-      <c r="L33" s="129"/>
+      <c r="E33" s="128"/>
+      <c r="F33" s="128"/>
+      <c r="G33" s="128"/>
+      <c r="H33" s="128"/>
+      <c r="I33" s="128"/>
+      <c r="J33" s="128"/>
+      <c r="K33" s="128"/>
+      <c r="L33" s="128"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="97"/>
@@ -6772,15 +6772,15 @@
       <c r="C34" s="81">
         <v>0</v>
       </c>
-      <c r="D34" s="128"/>
-      <c r="E34" s="128"/>
-      <c r="F34" s="128"/>
-      <c r="G34" s="128"/>
-      <c r="H34" s="128"/>
-      <c r="I34" s="128"/>
-      <c r="J34" s="128"/>
-      <c r="K34" s="128"/>
-      <c r="L34" s="128"/>
+      <c r="D34" s="127"/>
+      <c r="E34" s="127"/>
+      <c r="F34" s="127"/>
+      <c r="G34" s="127"/>
+      <c r="H34" s="127"/>
+      <c r="I34" s="127"/>
+      <c r="J34" s="127"/>
+      <c r="K34" s="127"/>
+      <c r="L34" s="127"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="97"/>
@@ -6788,15 +6788,15 @@
       <c r="C35" s="81">
         <v>0</v>
       </c>
-      <c r="D35" s="128"/>
-      <c r="E35" s="128"/>
-      <c r="F35" s="128"/>
-      <c r="G35" s="128"/>
-      <c r="H35" s="128"/>
-      <c r="I35" s="128"/>
-      <c r="J35" s="128"/>
-      <c r="K35" s="128"/>
-      <c r="L35" s="128"/>
+      <c r="D35" s="127"/>
+      <c r="E35" s="127"/>
+      <c r="F35" s="127"/>
+      <c r="G35" s="127"/>
+      <c r="H35" s="127"/>
+      <c r="I35" s="127"/>
+      <c r="J35" s="127"/>
+      <c r="K35" s="127"/>
+      <c r="L35" s="127"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="97"/>
@@ -6804,15 +6804,15 @@
       <c r="C36" s="81">
         <v>0</v>
       </c>
-      <c r="D36" s="128"/>
-      <c r="E36" s="128"/>
-      <c r="F36" s="128"/>
-      <c r="G36" s="128"/>
-      <c r="H36" s="128"/>
-      <c r="I36" s="128"/>
-      <c r="J36" s="128"/>
-      <c r="K36" s="128"/>
-      <c r="L36" s="128"/>
+      <c r="D36" s="127"/>
+      <c r="E36" s="127"/>
+      <c r="F36" s="127"/>
+      <c r="G36" s="127"/>
+      <c r="H36" s="127"/>
+      <c r="I36" s="127"/>
+      <c r="J36" s="127"/>
+      <c r="K36" s="127"/>
+      <c r="L36" s="127"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="77">
@@ -6859,17 +6859,17 @@
       <c r="C39" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="D39" s="129" t="s">
+      <c r="D39" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="129"/>
-      <c r="F39" s="129"/>
-      <c r="G39" s="129"/>
-      <c r="H39" s="129"/>
-      <c r="I39" s="129"/>
-      <c r="J39" s="129"/>
-      <c r="K39" s="129"/>
-      <c r="L39" s="129"/>
+      <c r="E39" s="128"/>
+      <c r="F39" s="128"/>
+      <c r="G39" s="128"/>
+      <c r="H39" s="128"/>
+      <c r="I39" s="128"/>
+      <c r="J39" s="128"/>
+      <c r="K39" s="128"/>
+      <c r="L39" s="128"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="97"/>
@@ -6877,15 +6877,15 @@
       <c r="C40" s="81">
         <v>0</v>
       </c>
-      <c r="D40" s="128"/>
-      <c r="E40" s="128"/>
-      <c r="F40" s="128"/>
-      <c r="G40" s="128"/>
-      <c r="H40" s="128"/>
-      <c r="I40" s="128"/>
-      <c r="J40" s="128"/>
-      <c r="K40" s="128"/>
-      <c r="L40" s="128"/>
+      <c r="D40" s="127"/>
+      <c r="E40" s="127"/>
+      <c r="F40" s="127"/>
+      <c r="G40" s="127"/>
+      <c r="H40" s="127"/>
+      <c r="I40" s="127"/>
+      <c r="J40" s="127"/>
+      <c r="K40" s="127"/>
+      <c r="L40" s="127"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="97"/>
@@ -6893,15 +6893,15 @@
       <c r="C41" s="81">
         <v>0</v>
       </c>
-      <c r="D41" s="128"/>
-      <c r="E41" s="128"/>
-      <c r="F41" s="128"/>
-      <c r="G41" s="128"/>
-      <c r="H41" s="128"/>
-      <c r="I41" s="128"/>
-      <c r="J41" s="128"/>
-      <c r="K41" s="128"/>
-      <c r="L41" s="128"/>
+      <c r="D41" s="127"/>
+      <c r="E41" s="127"/>
+      <c r="F41" s="127"/>
+      <c r="G41" s="127"/>
+      <c r="H41" s="127"/>
+      <c r="I41" s="127"/>
+      <c r="J41" s="127"/>
+      <c r="K41" s="127"/>
+      <c r="L41" s="127"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="97"/>
@@ -6909,15 +6909,15 @@
       <c r="C42" s="81">
         <v>0</v>
       </c>
-      <c r="D42" s="128"/>
-      <c r="E42" s="128"/>
-      <c r="F42" s="128"/>
-      <c r="G42" s="128"/>
-      <c r="H42" s="128"/>
-      <c r="I42" s="128"/>
-      <c r="J42" s="128"/>
-      <c r="K42" s="128"/>
-      <c r="L42" s="128"/>
+      <c r="D42" s="127"/>
+      <c r="E42" s="127"/>
+      <c r="F42" s="127"/>
+      <c r="G42" s="127"/>
+      <c r="H42" s="127"/>
+      <c r="I42" s="127"/>
+      <c r="J42" s="127"/>
+      <c r="K42" s="127"/>
+      <c r="L42" s="127"/>
     </row>
     <row r="43" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="95">
@@ -6930,18 +6930,33 @@
         <f>SUM(C40:C42)</f>
         <v>0</v>
       </c>
-      <c r="D43" s="132"/>
-      <c r="E43" s="132"/>
-      <c r="F43" s="132"/>
-      <c r="G43" s="132"/>
-      <c r="H43" s="132"/>
-      <c r="I43" s="132"/>
-      <c r="J43" s="132"/>
-      <c r="K43" s="132"/>
-      <c r="L43" s="132"/>
+      <c r="D43" s="129"/>
+      <c r="E43" s="129"/>
+      <c r="F43" s="129"/>
+      <c r="G43" s="129"/>
+      <c r="H43" s="129"/>
+      <c r="I43" s="129"/>
+      <c r="J43" s="129"/>
+      <c r="K43" s="129"/>
+      <c r="L43" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A6:L8"/>
+    <mergeCell ref="D10:L10"/>
+    <mergeCell ref="D11:L11"/>
+    <mergeCell ref="D12:L12"/>
+    <mergeCell ref="D15:L15"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B5:L5"/>
+    <mergeCell ref="D30:L30"/>
+    <mergeCell ref="D34:L34"/>
+    <mergeCell ref="D35:L35"/>
+    <mergeCell ref="D29:L29"/>
+    <mergeCell ref="D9:L9"/>
     <mergeCell ref="D36:L36"/>
     <mergeCell ref="D39:L39"/>
     <mergeCell ref="D33:L33"/>
@@ -6958,21 +6973,6 @@
     <mergeCell ref="D42:L42"/>
     <mergeCell ref="D40:L40"/>
     <mergeCell ref="D41:L41"/>
-    <mergeCell ref="D30:L30"/>
-    <mergeCell ref="D34:L34"/>
-    <mergeCell ref="D35:L35"/>
-    <mergeCell ref="D29:L29"/>
-    <mergeCell ref="D9:L9"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="B5:L5"/>
-    <mergeCell ref="A6:L8"/>
-    <mergeCell ref="D10:L10"/>
-    <mergeCell ref="D11:L11"/>
-    <mergeCell ref="D12:L12"/>
-    <mergeCell ref="D15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="63" orientation="portrait" r:id="rId1"/>

</xml_diff>